<commit_message>
Add color in compare_rule
</commit_message>
<xml_diff>
--- a/output/freight_outward.xlsx
+++ b/output/freight_outward.xlsx
@@ -378,10 +378,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="n">
+        <v>827.432609597449</v>
+      </c>
+      <c r="B1" s="0" t="n">
         <v>778.5150842666409</v>
-      </c>
-      <c r="B1" s="0" t="n">
-        <v>827.432609597449</v>
       </c>
       <c r="C1" s="0" t="n">
         <v>778.5150842666409</v>
@@ -680,10 +680,10 @@
     </row>
     <row r="2">
       <c r="A2" s="0" t="n">
-        <v>802.6012508000001</v>
+        <v>853.0322158641276</v>
       </c>
       <c r="B2" s="0" t="n">
-        <v>802.6012508</v>
+        <v>755.1517466818966</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>755.1517466818966</v>
@@ -985,7 +985,7 @@
         <v>827.4326095974491</v>
       </c>
       <c r="B3" s="0" t="n">
-        <v>827.432609597449</v>
+        <v>732.4895458562594</v>
       </c>
       <c r="C3" s="0" t="n">
         <v>778.515084266641</v>
@@ -1287,7 +1287,7 @@
         <v>802.6012508000001</v>
       </c>
       <c r="B4" s="0" t="n">
-        <v>802.6012508</v>
+        <v>710.5074405856125</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>802.6012508000002</v>
@@ -1586,10 +1586,10 @@
     </row>
     <row r="5">
       <c r="A5" s="0" t="n">
-        <v>827.4326095974491</v>
+        <v>778.515084266641</v>
       </c>
       <c r="B5" s="0" t="n">
-        <v>827.432609597449</v>
+        <v>689.1850211150747</v>
       </c>
       <c r="C5" s="0" t="n">
         <v>778.5150842666411</v>
@@ -1888,10 +1888,10 @@
     </row>
     <row r="6">
       <c r="A6" s="0" t="n">
-        <v>802.6012508000001</v>
+        <v>755.1517466818967</v>
       </c>
       <c r="B6" s="0" t="n">
-        <v>802.6012508</v>
+        <v>710.5074405856125</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>755.1517466818968</v>
@@ -2190,10 +2190,10 @@
     </row>
     <row r="7">
       <c r="A7" s="0" t="n">
-        <v>778.515084266641</v>
+        <v>778.5150842666411</v>
       </c>
       <c r="B7" s="0" t="n">
-        <v>827.432609597449</v>
+        <v>732.4895458562594</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>732.4895458562596</v>
@@ -2492,10 +2492,10 @@
     </row>
     <row r="8">
       <c r="A8" s="0" t="n">
-        <v>802.6012508000002</v>
+        <v>755.1517466818968</v>
       </c>
       <c r="B8" s="0" t="n">
-        <v>802.6012508</v>
+        <v>755.1517466818966</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>755.1517466818968</v>
@@ -2794,10 +2794,10 @@
     </row>
     <row r="9">
       <c r="A9" s="0" t="n">
-        <v>778.5150842666411</v>
+        <v>732.4895458562596</v>
       </c>
       <c r="B9" s="0" t="n">
-        <v>827.432609597449</v>
+        <v>732.4895458562594</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>732.4895458562596</v>
@@ -3099,7 +3099,7 @@
         <v>755.1517466818968</v>
       </c>
       <c r="B10" s="0" t="n">
-        <v>802.6012508</v>
+        <v>710.5074405856125</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>710.5074405856127</v>
@@ -3398,10 +3398,10 @@
     </row>
     <row r="11">
       <c r="A11" s="0" t="n">
-        <v>732.4895458562596</v>
+        <v>778.5150842666412</v>
       </c>
       <c r="B11" s="0" t="n">
-        <v>778.5150842666409</v>
+        <v>732.4895458562594</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>732.4895458562596</v>
@@ -3700,7 +3700,7 @@
     </row>
     <row r="12">
       <c r="A12" s="0" t="n">
-        <v>710.5074405856127</v>
+        <v>755.151746681897</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>755.1517466818966</v>
@@ -4002,10 +4002,10 @@
     </row>
     <row r="13">
       <c r="A13" s="0" t="n">
-        <v>732.4895458562596</v>
+        <v>778.5150842666413</v>
       </c>
       <c r="B13" s="0" t="n">
-        <v>732.4895458562594</v>
+        <v>778.515084266641</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>732.4895458562596</v>
@@ -4304,10 +4304,10 @@
     </row>
     <row r="14">
       <c r="A14" s="0" t="n">
-        <v>710.5074405856127</v>
+        <v>755.1517466818971</v>
       </c>
       <c r="B14" s="0" t="n">
-        <v>755.1517466818966</v>
+        <v>755.1517466818967</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>710.5074405856127</v>
@@ -4606,10 +4606,10 @@
     </row>
     <row r="15">
       <c r="A15" s="0" t="n">
-        <v>732.4895458562596</v>
+        <v>778.5150842666415</v>
       </c>
       <c r="B15" s="0" t="n">
-        <v>732.4895458562594</v>
+        <v>778.5150842666411</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>732.4895458562596</v>
@@ -4908,10 +4908,10 @@
     </row>
     <row r="16">
       <c r="A16" s="0" t="n">
-        <v>710.5074405856127</v>
+        <v>755.1517466818972</v>
       </c>
       <c r="B16" s="0" t="n">
-        <v>755.1517466818966</v>
+        <v>755.1517466818968</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>710.5074405856127</v>
@@ -5210,10 +5210,10 @@
     </row>
     <row r="17">
       <c r="A17" s="0" t="n">
-        <v>689.185021115075</v>
+        <v>778.5150842666416</v>
       </c>
       <c r="B17" s="0" t="n">
-        <v>732.4895458562594</v>
+        <v>732.4895458562596</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>732.4895458562596</v>
@@ -5512,10 +5512,10 @@
     </row>
     <row r="18">
       <c r="A18" s="0" t="n">
-        <v>668.5024901891285</v>
+        <v>755.1517466818973</v>
       </c>
       <c r="B18" s="0" t="n">
-        <v>710.5074405856125</v>
+        <v>710.5074405856127</v>
       </c>
       <c r="C18" s="0" t="n">
         <v>710.5074405856127</v>
@@ -5814,10 +5814,10 @@
     </row>
     <row r="19">
       <c r="A19" s="0" t="n">
-        <v>689.1850211150751</v>
+        <v>732.4895458562601</v>
       </c>
       <c r="B19" s="0" t="n">
-        <v>689.1850211150747</v>
+        <v>732.4895458562596</v>
       </c>
       <c r="C19" s="0" t="n">
         <v>689.185021115075</v>
@@ -6116,10 +6116,10 @@
     </row>
     <row r="20">
       <c r="A20" s="0" t="n">
-        <v>710.5074405856128</v>
+        <v>710.5074405856132</v>
       </c>
       <c r="B20" s="0" t="n">
-        <v>668.5024901891283</v>
+        <v>710.5074405856127</v>
       </c>
       <c r="C20" s="0" t="n">
         <v>668.5024901891285</v>
@@ -6418,10 +6418,10 @@
     </row>
     <row r="21">
       <c r="A21" s="0" t="n">
-        <v>689.1850211150751</v>
+        <v>689.1850211150754</v>
       </c>
       <c r="B21" s="0" t="n">
-        <v>648.4406446704337</v>
+        <v>689.185021115075</v>
       </c>
       <c r="C21" s="0" t="n">
         <v>648.4406446704339</v>
@@ -6720,10 +6720,10 @@
     </row>
     <row r="22">
       <c r="A22" s="0" t="n">
-        <v>668.5024901891286</v>
+        <v>668.5024901891289</v>
       </c>
       <c r="B22" s="0" t="n">
-        <v>628.9808577102676</v>
+        <v>668.5024901891285</v>
       </c>
       <c r="C22" s="0" t="n">
         <v>628.9808577102679</v>
@@ -7022,10 +7022,10 @@
     </row>
     <row r="23">
       <c r="A23" s="0" t="n">
-        <v>689.1850211150752</v>
+        <v>648.4406446704344</v>
       </c>
       <c r="B23" s="0" t="n">
-        <v>648.4406446704338</v>
+        <v>689.1850211150751</v>
       </c>
       <c r="C23" s="0" t="n">
         <v>610.1050614540274</v>
@@ -7324,10 +7324,10 @@
     </row>
     <row r="24">
       <c r="A24" s="0" t="n">
-        <v>710.5074405856129</v>
+        <v>628.9808577102683</v>
       </c>
       <c r="B24" s="0" t="n">
-        <v>628.9808577102677</v>
+        <v>710.5074405856128</v>
       </c>
       <c r="C24" s="0" t="n">
         <v>591.7957302657449</v>
@@ -7626,10 +7626,10 @@
     </row>
     <row r="25">
       <c r="A25" s="0" t="n">
-        <v>689.1850211150752</v>
+        <v>610.1050614540278</v>
       </c>
       <c r="B25" s="0" t="n">
-        <v>648.4406446704339</v>
+        <v>732.4895458562597</v>
       </c>
       <c r="C25" s="0" t="n">
         <v>574.0358644560371</v>
@@ -7928,10 +7928,10 @@
     </row>
     <row r="26">
       <c r="A26" s="0" t="n">
-        <v>710.5074405856129</v>
+        <v>628.9808577102684</v>
       </c>
       <c r="B26" s="0" t="n">
-        <v>628.9808577102679</v>
+        <v>755.151746681897</v>
       </c>
       <c r="C26" s="0" t="n">
         <v>556.8089744983808</v>
@@ -8230,10 +8230,10 @@
     </row>
     <row r="27">
       <c r="A27" s="0" t="n">
-        <v>689.1850211150752</v>
+        <v>610.1050614540279</v>
       </c>
       <c r="B27" s="0" t="n">
-        <v>648.440644670434</v>
+        <v>778.5150842666413</v>
       </c>
       <c r="C27" s="0" t="n">
         <v>574.0358644560372</v>
@@ -8532,10 +8532,10 @@
     </row>
     <row r="28">
       <c r="A28" s="0" t="n">
-        <v>710.5074405856129</v>
+        <v>591.7957302657454</v>
       </c>
       <c r="B28" s="0" t="n">
-        <v>668.5024901891287</v>
+        <v>755.1517466818971</v>
       </c>
       <c r="C28" s="0" t="n">
         <v>591.795730265745</v>
@@ -8834,10 +8834,10 @@
     </row>
     <row r="29">
       <c r="A29" s="0" t="n">
-        <v>689.1850211150752</v>
+        <v>574.0358644560376</v>
       </c>
       <c r="B29" s="0" t="n">
-        <v>689.1850211150753</v>
+        <v>732.4895458562598</v>
       </c>
       <c r="C29" s="0" t="n">
         <v>610.1050614540276</v>
@@ -9136,10 +9136,10 @@
     </row>
     <row r="30">
       <c r="A30" s="0" t="n">
-        <v>710.5074405856129</v>
+        <v>591.7957302657455</v>
       </c>
       <c r="B30" s="0" t="n">
-        <v>668.5024901891288</v>
+        <v>755.1517466818971</v>
       </c>
       <c r="C30" s="0" t="n">
         <v>591.7957302657451</v>
@@ -9438,10 +9438,10 @@
     </row>
     <row r="31">
       <c r="A31" s="0" t="n">
-        <v>732.48954585626</v>
+        <v>610.1050614540281</v>
       </c>
       <c r="B31" s="0" t="n">
-        <v>648.4406446704343</v>
+        <v>732.4895458562598</v>
       </c>
       <c r="C31" s="0" t="n">
         <v>610.1050614540277</v>
@@ -9740,10 +9740,10 @@
     </row>
     <row r="32">
       <c r="A32" s="0" t="n">
-        <v>755.1517466818972</v>
+        <v>628.9808577102688</v>
       </c>
       <c r="B32" s="0" t="n">
-        <v>668.5024901891289</v>
+        <v>710.5074405856129</v>
       </c>
       <c r="C32" s="0" t="n">
         <v>591.7957302657452</v>
@@ -10042,10 +10042,10 @@
     </row>
     <row r="33">
       <c r="A33" s="0" t="n">
-        <v>778.5150842666416</v>
+        <v>610.1050614540283</v>
       </c>
       <c r="B33" s="0" t="n">
-        <v>689.1850211150755</v>
+        <v>689.1850211150752</v>
       </c>
       <c r="C33" s="0" t="n">
         <v>610.1050614540278</v>
@@ -10344,10 +10344,10 @@
     </row>
     <row r="34">
       <c r="A34" s="0" t="n">
-        <v>802.6012508000008</v>
+        <v>628.9808577102689</v>
       </c>
       <c r="B34" s="0" t="n">
-        <v>710.5074405856133</v>
+        <v>668.5024901891287</v>
       </c>
       <c r="C34" s="0" t="n">
         <v>591.7957302657453</v>
@@ -10646,10 +10646,10 @@
     </row>
     <row r="35">
       <c r="A35" s="0" t="n">
-        <v>778.5150842666417</v>
+        <v>610.1050614540284</v>
       </c>
       <c r="B35" s="0" t="n">
-        <v>732.4895458562603</v>
+        <v>689.1850211150753</v>
       </c>
       <c r="C35" s="0" t="n">
         <v>574.0358644560375</v>
@@ -10948,10 +10948,10 @@
     </row>
     <row r="36">
       <c r="A36" s="0" t="n">
-        <v>802.6012508000009</v>
+        <v>628.980857710269</v>
       </c>
       <c r="B36" s="0" t="n">
-        <v>755.1517466818975</v>
+        <v>668.5024901891288</v>
       </c>
       <c r="C36" s="0" t="n">
         <v>556.8089744983813</v>
@@ -11250,10 +11250,10 @@
     </row>
     <row r="37">
       <c r="A37" s="0" t="n">
-        <v>778.5150842666418</v>
+        <v>610.1050614540285</v>
       </c>
       <c r="B37" s="0" t="n">
-        <v>732.4895458562603</v>
+        <v>648.4406446704343</v>
       </c>
       <c r="C37" s="0" t="n">
         <v>574.0358644560376</v>
@@ -11552,10 +11552,10 @@
     </row>
     <row r="38">
       <c r="A38" s="0" t="n">
-        <v>802.601250800001</v>
+        <v>628.9808577102691</v>
       </c>
       <c r="B38" s="0" t="n">
-        <v>755.1517466818975</v>
+        <v>628.9808577102682</v>
       </c>
       <c r="C38" s="0" t="n">
         <v>556.8089744983814</v>
@@ -11854,10 +11854,10 @@
     </row>
     <row r="39">
       <c r="A39" s="0" t="n">
-        <v>827.4326095974501</v>
+        <v>610.1050614540286</v>
       </c>
       <c r="B39" s="0" t="n">
-        <v>778.5150842666419</v>
+        <v>648.4406446704344</v>
       </c>
       <c r="C39" s="0" t="n">
         <v>574.0358644560378</v>
@@ -12156,10 +12156,10 @@
     </row>
     <row r="40">
       <c r="A40" s="0" t="n">
-        <v>802.6012508000011</v>
+        <v>628.9808577102692</v>
       </c>
       <c r="B40" s="0" t="n">
-        <v>802.6012508000011</v>
+        <v>628.9808577102683</v>
       </c>
       <c r="C40" s="0" t="n">
         <v>556.8089744983814</v>
@@ -12458,10 +12458,10 @@
     </row>
     <row r="41">
       <c r="A41" s="0" t="n">
-        <v>827.4326095974502</v>
+        <v>610.1050614540287</v>
       </c>
       <c r="B41" s="0" t="n">
-        <v>778.515084266642</v>
+        <v>648.4406446704345</v>
       </c>
       <c r="C41" s="0" t="n">
         <v>574.0358644560378</v>
@@ -12760,10 +12760,10 @@
     </row>
     <row r="42">
       <c r="A42" s="0" t="n">
-        <v>802.6012508000013</v>
+        <v>591.7957302657461</v>
       </c>
       <c r="B42" s="0" t="n">
-        <v>755.1517466818976</v>
+        <v>628.9808577102684</v>
       </c>
       <c r="C42" s="0" t="n">
         <v>556.8089744983814</v>
@@ -13062,10 +13062,10 @@
     </row>
     <row r="43">
       <c r="A43" s="0" t="n">
-        <v>827.4326095974503</v>
+        <v>574.0358644560383</v>
       </c>
       <c r="B43" s="0" t="n">
-        <v>778.515084266642</v>
+        <v>648.4406446704346</v>
       </c>
       <c r="C43" s="0" t="n">
         <v>540.0990657190604</v>
@@ -13364,10 +13364,10 @@
     </row>
     <row r="44">
       <c r="A44" s="0" t="n">
-        <v>853.0322158641291</v>
+        <v>556.808974498382</v>
       </c>
       <c r="B44" s="0" t="n">
-        <v>802.6012508000013</v>
+        <v>668.5024901891293</v>
       </c>
       <c r="C44" s="0" t="n">
         <v>523.8906234465693</v>
@@ -13666,10 +13666,10 @@
     </row>
     <row r="45">
       <c r="A45" s="0" t="n">
-        <v>827.4326095974504</v>
+        <v>540.0990657190609</v>
       </c>
       <c r="B45" s="0" t="n">
-        <v>827.4326095974503</v>
+        <v>648.4406446704347</v>
       </c>
       <c r="C45" s="0" t="n">
         <v>540.0990657190605</v>
@@ -13968,10 +13968,10 @@
     </row>
     <row r="46">
       <c r="A46" s="0" t="n">
-        <v>802.6012508000015</v>
+        <v>523.8906234465699</v>
       </c>
       <c r="B46" s="0" t="n">
-        <v>853.0322158641291</v>
+        <v>668.5024901891294</v>
       </c>
       <c r="C46" s="0" t="n">
         <v>523.8906234465694</v>
@@ -14270,10 +14270,10 @@
     </row>
     <row r="47">
       <c r="A47" s="0" t="n">
-        <v>827.4326095974506</v>
+        <v>508.168598606686</v>
       </c>
       <c r="B47" s="0" t="n">
-        <v>827.4326095974504</v>
+        <v>648.4406446704348</v>
       </c>
       <c r="C47" s="0" t="n">
         <v>540.0990657190606</v>
@@ -14572,10 +14572,10 @@
     </row>
     <row r="48">
       <c r="A48" s="0" t="n">
-        <v>802.6012508000016</v>
+        <v>523.8906234465699</v>
       </c>
       <c r="B48" s="0" t="n">
-        <v>802.6012508000015</v>
+        <v>668.5024901891295</v>
       </c>
       <c r="C48" s="0" t="n">
         <v>556.8089744983816</v>
@@ -14874,10 +14874,10 @@
     </row>
     <row r="49">
       <c r="A49" s="0" t="n">
-        <v>778.5150842666425</v>
+        <v>540.0990657190611</v>
       </c>
       <c r="B49" s="0" t="n">
-        <v>827.4326095974506</v>
+        <v>689.1850211150761</v>
       </c>
       <c r="C49" s="0" t="n">
         <v>540.0990657190606</v>
@@ -15176,10 +15176,10 @@
     </row>
     <row r="50">
       <c r="A50" s="0" t="n">
-        <v>755.1517466818981</v>
+        <v>556.8089744983821</v>
       </c>
       <c r="B50" s="0" t="n">
-        <v>853.0322158641293</v>
+        <v>710.5074405856139</v>
       </c>
       <c r="C50" s="0" t="n">
         <v>523.8906234465695</v>
@@ -15478,10 +15478,10 @@
     </row>
     <row r="51">
       <c r="A51" s="0" t="n">
-        <v>778.5150842666425</v>
+        <v>574.0358644560384</v>
       </c>
       <c r="B51" s="0" t="n">
-        <v>879.4238381009397</v>
+        <v>689.1850211150762</v>
       </c>
       <c r="C51" s="0" t="n">
         <v>508.1685986066857</v>
@@ -15780,10 +15780,10 @@
     </row>
     <row r="52">
       <c r="A52" s="0" t="n">
-        <v>755.1517466818981</v>
+        <v>591.7957302657463</v>
       </c>
       <c r="B52" s="0" t="n">
-        <v>906.6319801729184</v>
+        <v>710.5074405856141</v>
       </c>
       <c r="C52" s="0" t="n">
         <v>492.9183937498353</v>
@@ -16082,10 +16082,10 @@
     </row>
     <row r="53">
       <c r="A53" s="0" t="n">
-        <v>732.4895458562609</v>
+        <v>610.1050614540289</v>
       </c>
       <c r="B53" s="0" t="n">
-        <v>879.4238381009399</v>
+        <v>732.4895458562611</v>
       </c>
       <c r="C53" s="0" t="n">
         <v>478.1258494977794</v>
@@ -16384,10 +16384,10 @@
     </row>
     <row r="54">
       <c r="A54" s="0" t="n">
-        <v>710.5074405856139</v>
+        <v>591.7957302657463</v>
       </c>
       <c r="B54" s="0" t="n">
-        <v>853.0322158641295</v>
+        <v>710.5074405856142</v>
       </c>
       <c r="C54" s="0" t="n">
         <v>463.777231397037</v>
@@ -16686,10 +16686,10 @@
     </row>
     <row r="55">
       <c r="A55" s="0" t="n">
-        <v>689.1850211150762</v>
+        <v>610.1050614540289</v>
       </c>
       <c r="B55" s="0" t="n">
-        <v>879.42383810094</v>
+        <v>689.1850211150764</v>
       </c>
       <c r="C55" s="0" t="n">
         <v>478.1258494977794</v>
@@ -16988,10 +16988,10 @@
     </row>
     <row r="56">
       <c r="A56" s="0" t="n">
-        <v>710.5074405856141</v>
+        <v>591.7957302657463</v>
       </c>
       <c r="B56" s="0" t="n">
-        <v>906.6319801729186</v>
+        <v>668.50249018913</v>
       </c>
       <c r="C56" s="0" t="n">
         <v>463.7772313970371</v>
@@ -17290,10 +17290,10 @@
     </row>
     <row r="57">
       <c r="A57" s="0" t="n">
-        <v>689.1850211150763</v>
+        <v>574.0358644560386</v>
       </c>
       <c r="B57" s="0" t="n">
-        <v>934.6819040603726</v>
+        <v>648.4406446704354</v>
       </c>
       <c r="C57" s="0" t="n">
         <v>449.8592171668389</v>
@@ -17592,10 +17592,10 @@
     </row>
     <row r="58">
       <c r="A58" s="0" t="n">
-        <v>710.5074405856142</v>
+        <v>556.8089744983822</v>
       </c>
       <c r="B58" s="0" t="n">
-        <v>963.599653313905</v>
+        <v>628.9808577102693</v>
       </c>
       <c r="C58" s="0" t="n">
         <v>436.3588843297709</v>
@@ -17894,10 +17894,10 @@
     </row>
     <row r="59">
       <c r="A59" s="0" t="n">
-        <v>689.1850211150764</v>
+        <v>574.0358644560386</v>
       </c>
       <c r="B59" s="0" t="n">
-        <v>993.4120772351051</v>
+        <v>648.4406446704355</v>
       </c>
       <c r="C59" s="0" t="n">
         <v>449.859217166839</v>
@@ -18196,10 +18196,10 @@
     </row>
     <row r="60">
       <c r="A60" s="0" t="n">
-        <v>668.50249018913</v>
+        <v>556.8089744983822</v>
       </c>
       <c r="B60" s="0" t="n">
-        <v>1024.146855805355</v>
+        <v>628.9808577102694</v>
       </c>
       <c r="C60" s="0" t="n">
         <v>463.7772313970372</v>
@@ -18498,10 +18498,10 @@
     </row>
     <row r="61">
       <c r="A61" s="0" t="n">
-        <v>689.1850211150766</v>
+        <v>540.0990657190612</v>
       </c>
       <c r="B61" s="0" t="n">
-        <v>1055.832525385902</v>
+        <v>610.1050614540289</v>
       </c>
       <c r="C61" s="0" t="n">
         <v>449.859217166839</v>
@@ -18800,10 +18800,10 @@
     </row>
     <row r="62">
       <c r="A62" s="0" t="n">
-        <v>668.5024901891301</v>
+        <v>523.8906234465701</v>
       </c>
       <c r="B62" s="0" t="n">
-        <v>1088.498505213047</v>
+        <v>591.7957302657463</v>
       </c>
       <c r="C62" s="0" t="n">
         <v>463.7772313970373</v>
@@ -19102,10 +19102,10 @@
     </row>
     <row r="63">
       <c r="A63" s="0" t="n">
-        <v>689.1850211150767</v>
+        <v>508.1685986066863</v>
       </c>
       <c r="B63" s="0" t="n">
-        <v>1122.175124713067</v>
+        <v>610.1050614540289</v>
       </c>
       <c r="C63" s="0" t="n">
         <v>449.8592171668391</v>
@@ -19404,10 +19404,10 @@
     </row>
     <row r="64">
       <c r="A64" s="0" t="n">
-        <v>710.5074405856145</v>
+        <v>523.8906234465701</v>
       </c>
       <c r="B64" s="0" t="n">
-        <v>1156.893651662218</v>
+        <v>591.7957302657463</v>
       </c>
       <c r="C64" s="0" t="n">
         <v>436.3588843297711</v>
@@ -19706,10 +19706,10 @@
     </row>
     <row r="65">
       <c r="A65" s="0" t="n">
-        <v>732.4895458562615</v>
+        <v>508.1685986066863</v>
       </c>
       <c r="B65" s="0" t="n">
-        <v>1192.686321217968</v>
+        <v>610.1050614540289</v>
       </c>
       <c r="C65" s="0" t="n">
         <v>423.263698213625</v>
@@ -20008,10 +20008,10 @@
     </row>
     <row r="66">
       <c r="A66" s="0" t="n">
-        <v>755.1517466818989</v>
+        <v>523.8906234465701</v>
       </c>
       <c r="B66" s="0" t="n">
-        <v>1229.586365848415</v>
+        <v>628.9808577102696</v>
       </c>
       <c r="C66" s="0" t="n">
         <v>410.5615003133139</v>
@@ -20310,10 +20310,10 @@
     </row>
     <row r="67">
       <c r="A67" s="0" t="n">
-        <v>732.4895458562617</v>
+        <v>508.1685986066863</v>
       </c>
       <c r="B67" s="0" t="n">
-        <v>1192.686321217968</v>
+        <v>610.1050614540291</v>
       </c>
       <c r="C67" s="0" t="n">
         <v>398.2404970020489</v>
@@ -20612,10 +20612,10 @@
     </row>
     <row r="68">
       <c r="A68" s="0" t="n">
-        <v>755.151746681899</v>
+        <v>492.9183937498358</v>
       </c>
       <c r="B68" s="0" t="n">
-        <v>1229.586365848415</v>
+        <v>628.9808577102697</v>
       </c>
       <c r="C68" s="0" t="n">
         <v>386.2892485812944</v>
@@ -20914,10 +20914,10 @@
     </row>
     <row r="69">
       <c r="A69" s="0" t="n">
-        <v>732.4895458562618</v>
+        <v>478.1258494977799</v>
       </c>
       <c r="B69" s="0" t="n">
-        <v>1267.628046187687</v>
+        <v>648.4406446704359</v>
       </c>
       <c r="C69" s="0" t="n">
         <v>398.2404970020489</v>
@@ -21216,10 +21216,10 @@
     </row>
     <row r="70">
       <c r="A70" s="0" t="n">
-        <v>755.1517466818991</v>
+        <v>463.7772313970376</v>
       </c>
       <c r="B70" s="0" t="n">
-        <v>1306.846682845954</v>
+        <v>668.5024901891305</v>
       </c>
       <c r="C70" s="0" t="n">
         <v>410.561500313314</v>
@@ -21518,10 +21518,10 @@
     </row>
     <row r="71">
       <c r="A71" s="0" t="n">
-        <v>778.5150842666436</v>
+        <v>449.8592171668394</v>
       </c>
       <c r="B71" s="0" t="n">
-        <v>1347.278689203605</v>
+        <v>689.1850211150771</v>
       </c>
       <c r="C71" s="0" t="n">
         <v>423.2636982136252</v>
@@ -21820,10 +21820,10 @@
     </row>
     <row r="72">
       <c r="A72" s="0" t="n">
-        <v>802.601250800003</v>
+        <v>436.3588843297715</v>
       </c>
       <c r="B72" s="0" t="n">
-        <v>1388.961605220027</v>
+        <v>668.5024901891305</v>
       </c>
       <c r="C72" s="0" t="n">
         <v>410.5615003133141</v>
@@ -22122,10 +22122,10 @@
     </row>
     <row r="73">
       <c r="A73" s="0" t="n">
-        <v>827.432609597452</v>
+        <v>423.2636982136253</v>
       </c>
       <c r="B73" s="0" t="n">
-        <v>1347.278689203605</v>
+        <v>648.4406446704359</v>
       </c>
       <c r="C73" s="0" t="n">
         <v>398.240497002049</v>
@@ -22424,10 +22424,10 @@
     </row>
     <row r="74">
       <c r="A74" s="0" t="n">
-        <v>802.6012508000031</v>
+        <v>410.5615003133142</v>
       </c>
       <c r="B74" s="0" t="n">
-        <v>1388.961605220027</v>
+        <v>668.5024901891305</v>
       </c>
       <c r="C74" s="0" t="n">
         <v>386.2892485812946</v>
@@ -22726,10 +22726,10 @@
     </row>
     <row r="75">
       <c r="A75" s="0" t="n">
-        <v>778.5150842666438</v>
+        <v>398.2404970020492</v>
       </c>
       <c r="B75" s="0" t="n">
-        <v>1431.934132288382</v>
+        <v>689.1850211150771</v>
       </c>
       <c r="C75" s="0" t="n">
         <v>398.2404970020491</v>
@@ -23028,10 +23028,10 @@
     </row>
     <row r="76">
       <c r="A76" s="0" t="n">
-        <v>755.1517466818995</v>
+        <v>386.2892485812947</v>
       </c>
       <c r="B76" s="0" t="n">
-        <v>1388.961605220027</v>
+        <v>710.507440585615</v>
       </c>
       <c r="C76" s="0" t="n">
         <v>386.2892485812946</v>
@@ -23330,10 +23330,10 @@
     </row>
     <row r="77">
       <c r="A77" s="0" t="n">
-        <v>778.515084266644</v>
+        <v>398.2404970020492</v>
       </c>
       <c r="B77" s="0" t="n">
-        <v>1347.278689203605</v>
+        <v>689.1850211150772</v>
       </c>
       <c r="C77" s="0" t="n">
         <v>374.6966586593363</v>
@@ -23632,10 +23632,10 @@
     </row>
     <row r="78">
       <c r="A78" s="0" t="n">
-        <v>802.6012508000033</v>
+        <v>386.2892485812947</v>
       </c>
       <c r="B78" s="0" t="n">
-        <v>1388.961605220027</v>
+        <v>668.5024901891306</v>
       </c>
       <c r="C78" s="0" t="n">
         <v>363.451963848599</v>
@@ -23934,10 +23934,10 @@
     </row>
     <row r="79">
       <c r="A79" s="0" t="n">
-        <v>778.5150842666441</v>
+        <v>398.2404970020492</v>
       </c>
       <c r="B79" s="0" t="n">
-        <v>1347.278689203605</v>
+        <v>689.1850211150772</v>
       </c>
       <c r="C79" s="0" t="n">
         <v>352.5447237721501</v>
@@ -24236,10 +24236,10 @@
     </row>
     <row r="80">
       <c r="A80" s="0" t="n">
-        <v>802.6012508000034</v>
+        <v>386.2892485812947</v>
       </c>
       <c r="B80" s="0" t="n">
-        <v>1388.961605220027</v>
+        <v>710.5074405856151</v>
       </c>
       <c r="C80" s="0" t="n">
         <v>363.4519638485991</v>
@@ -24538,10 +24538,10 @@
     </row>
     <row r="81">
       <c r="A81" s="0" t="n">
-        <v>827.4326095974525</v>
+        <v>374.6966586593363</v>
       </c>
       <c r="B81" s="0" t="n">
-        <v>1431.934132288383</v>
+        <v>732.4895458562621</v>
       </c>
       <c r="C81" s="0" t="n">
         <v>352.5447237721502</v>
@@ -24840,10 +24840,10 @@
     </row>
     <row r="82">
       <c r="A82" s="0" t="n">
-        <v>853.0322158641312</v>
+        <v>363.4519638485991</v>
       </c>
       <c r="B82" s="0" t="n">
-        <v>1476.236169168745</v>
+        <v>710.5074405856152</v>
       </c>
       <c r="C82" s="0" t="n">
         <v>341.9648113701085</v>
@@ -25142,10 +25142,10 @@
     </row>
     <row r="83">
       <c r="A83" s="0" t="n">
-        <v>879.4238381009417</v>
+        <v>374.6966586593364</v>
       </c>
       <c r="B83" s="0" t="n">
-        <v>1431.934132288383</v>
+        <v>689.1850211150775</v>
       </c>
       <c r="C83" s="0" t="n">
         <v>352.5447237721502</v>
@@ -25444,10 +25444,10 @@
     </row>
     <row r="84">
       <c r="A84" s="0" t="n">
-        <v>853.0322158641312</v>
+        <v>386.2892485812947</v>
       </c>
       <c r="B84" s="0" t="n">
-        <v>1388.961605220027</v>
+        <v>668.5024901891309</v>
       </c>
       <c r="C84" s="0" t="n">
         <v>363.4519638485991</v>
@@ -25746,10 +25746,10 @@
     </row>
     <row r="85">
       <c r="A85" s="0" t="n">
-        <v>879.4238381009417</v>
+        <v>398.2404970020492</v>
       </c>
       <c r="B85" s="0" t="n">
-        <v>1431.934132288383</v>
+        <v>689.1850211150775</v>
       </c>
       <c r="C85" s="0" t="n">
         <v>374.6966586593364</v>
@@ -26048,10 +26048,10 @@
     </row>
     <row r="86">
       <c r="A86" s="0" t="n">
-        <v>906.6319801729203</v>
+        <v>386.2892485812947</v>
       </c>
       <c r="B86" s="0" t="n">
-        <v>1388.961605220027</v>
+        <v>668.5024901891309</v>
       </c>
       <c r="C86" s="0" t="n">
         <v>363.4519638485992</v>
@@ -26350,10 +26350,10 @@
     </row>
     <row r="87">
       <c r="A87" s="0" t="n">
-        <v>934.6819040603743</v>
+        <v>398.2404970020492</v>
       </c>
       <c r="B87" s="0" t="n">
-        <v>1347.278689203606</v>
+        <v>689.1850211150775</v>
       </c>
       <c r="C87" s="0" t="n">
         <v>374.6966586593365</v>
@@ -26652,10 +26652,10 @@
     </row>
     <row r="88">
       <c r="A88" s="0" t="n">
-        <v>963.5996533139069</v>
+        <v>386.2892485812947</v>
       </c>
       <c r="B88" s="0" t="n">
-        <v>1388.961605220028</v>
+        <v>668.5024901891309</v>
       </c>
       <c r="C88" s="0" t="n">
         <v>363.4519638485992</v>
@@ -26954,10 +26954,10 @@
     </row>
     <row r="89">
       <c r="A89" s="0" t="n">
-        <v>934.6819040603744</v>
+        <v>398.2404970020492</v>
       </c>
       <c r="B89" s="0" t="n">
-        <v>1431.934132288383</v>
+        <v>689.1850211150775</v>
       </c>
       <c r="C89" s="0" t="n">
         <v>352.5447237721503</v>
@@ -27256,10 +27256,10 @@
     </row>
     <row r="90">
       <c r="A90" s="0" t="n">
-        <v>963.599653313907</v>
+        <v>410.5615003133143</v>
       </c>
       <c r="B90" s="0" t="n">
-        <v>1388.961605220028</v>
+        <v>668.5024901891309</v>
       </c>
       <c r="C90" s="0" t="n">
         <v>341.9648113701086</v>
@@ -27558,10 +27558,10 @@
     </row>
     <row r="91">
       <c r="A91" s="0" t="n">
-        <v>934.6819040603746</v>
+        <v>398.2404970020493</v>
       </c>
       <c r="B91" s="0" t="n">
-        <v>1431.934132288383</v>
+        <v>689.1850211150775</v>
       </c>
       <c r="C91" s="0" t="n">
         <v>352.5447237721503</v>
@@ -27860,10 +27860,10 @@
     </row>
     <row r="92">
       <c r="A92" s="0" t="n">
-        <v>906.6319801729205</v>
+        <v>386.2892485812948</v>
       </c>
       <c r="B92" s="0" t="n">
-        <v>1388.961605220028</v>
+        <v>710.5074405856153</v>
       </c>
       <c r="C92" s="0" t="n">
         <v>363.4519638485993</v>
@@ -28162,10 +28162,10 @@
     </row>
     <row r="93">
       <c r="A93" s="0" t="n">
-        <v>879.4238381009419</v>
+        <v>374.6966586593364</v>
       </c>
       <c r="B93" s="0" t="n">
-        <v>1431.934132288383</v>
+        <v>689.1850211150776</v>
       </c>
       <c r="C93" s="0" t="n">
         <v>352.5447237721504</v>
@@ -28464,10 +28464,10 @@
     </row>
     <row r="94">
       <c r="A94" s="0" t="n">
-        <v>853.0322158641314</v>
+        <v>386.2892485812948</v>
       </c>
       <c r="B94" s="0" t="n">
-        <v>1388.961605220028</v>
+        <v>710.5074405856154</v>
       </c>
       <c r="C94" s="0" t="n">
         <v>363.4519638485993</v>
@@ -28766,10 +28766,10 @@
     </row>
     <row r="95">
       <c r="A95" s="0" t="n">
-        <v>879.4238381009419</v>
+        <v>374.6966586593365</v>
       </c>
       <c r="B95" s="0" t="n">
-        <v>1347.278689203606</v>
+        <v>689.1850211150777</v>
       </c>
       <c r="C95" s="0" t="n">
         <v>352.5447237721505</v>
@@ -29068,10 +29068,10 @@
     </row>
     <row r="96">
       <c r="A96" s="0" t="n">
-        <v>906.6319801729206</v>
+        <v>386.2892485812949</v>
       </c>
       <c r="B96" s="0" t="n">
-        <v>1306.846682845955</v>
+        <v>668.5024901891311</v>
       </c>
       <c r="C96" s="0" t="n">
         <v>341.9648113701087</v>
@@ -29370,10 +29370,10 @@
     </row>
     <row r="97">
       <c r="A97" s="0" t="n">
-        <v>934.6819040603748</v>
+        <v>398.2404970020494</v>
       </c>
       <c r="B97" s="0" t="n">
-        <v>1347.278689203606</v>
+        <v>648.4406446704364</v>
       </c>
       <c r="C97" s="0" t="n">
         <v>331.7024034969597</v>
@@ -29672,10 +29672,10 @@
     </row>
     <row r="98">
       <c r="A98" s="0" t="n">
-        <v>963.5996533139073</v>
+        <v>410.5615003133145</v>
       </c>
       <c r="B98" s="0" t="n">
-        <v>1306.846682845955</v>
+        <v>628.9808577102702</v>
       </c>
       <c r="C98" s="0" t="n">
         <v>321.7479718010463</v>
@@ -29974,10 +29974,10 @@
     </row>
     <row r="99">
       <c r="A99" s="0" t="n">
-        <v>934.6819040603749</v>
+        <v>423.2636982136256</v>
       </c>
       <c r="B99" s="0" t="n">
-        <v>1347.278689203606</v>
+        <v>648.4406446704364</v>
       </c>
       <c r="C99" s="0" t="n">
         <v>312.0922738777675</v>
@@ -30276,10 +30276,10 @@
     </row>
     <row r="100">
       <c r="A100" s="0" t="n">
-        <v>963.5996533139074</v>
+        <v>410.5615003133145</v>
       </c>
       <c r="B100" s="0" t="n">
-        <v>1306.846682845955</v>
+        <v>668.5024901891311</v>
       </c>
       <c r="C100" s="0" t="n">
         <v>302.7263446882704</v>
@@ -30578,10 +30578,10 @@
     </row>
     <row r="101">
       <c r="A101" s="0" t="n">
-        <v>993.4120772351076</v>
+        <v>423.2636982136256</v>
       </c>
       <c r="B101" s="0" t="n">
-        <v>1267.628046187689</v>
+        <v>689.1850211150777</v>
       </c>
       <c r="C101" s="0" t="n">
         <v>312.0922738777676</v>
@@ -30880,10 +30880,10 @@
     </row>
     <row r="102">
       <c r="A102" s="0" t="n">
-        <v>1024.146855805358</v>
+        <v>436.3588843297718</v>
       </c>
       <c r="B102" s="0" t="n">
-        <v>1306.846682845955</v>
+        <v>710.5074405856155</v>
       </c>
       <c r="C102" s="0" t="n">
         <v>302.7263446882704</v>
@@ -31182,10 +31182,10 @@
     </row>
     <row r="103">
       <c r="A103" s="0" t="n">
-        <v>993.4120772351079</v>
+        <v>423.2636982136257</v>
       </c>
       <c r="B103" s="0" t="n">
-        <v>1267.628046187689</v>
+        <v>732.4895458562626</v>
       </c>
       <c r="C103" s="0" t="n">
         <v>312.0922738777676</v>
@@ -31484,10 +31484,10 @@
     </row>
     <row r="104">
       <c r="A104" s="0" t="n">
-        <v>1024.146855805358</v>
+        <v>436.3588843297719</v>
       </c>
       <c r="B104" s="0" t="n">
-        <v>1306.846682845955</v>
+        <v>710.5074405856155</v>
       </c>
       <c r="C104" s="0" t="n">
         <v>302.7263446882705</v>
@@ -31786,10 +31786,10 @@
     </row>
     <row r="105">
       <c r="A105" s="0" t="n">
-        <v>1055.832525385905</v>
+        <v>423.2636982136257</v>
       </c>
       <c r="B105" s="0" t="n">
-        <v>1267.628046187689</v>
+        <v>689.1850211150778</v>
       </c>
       <c r="C105" s="0" t="n">
         <v>293.6414882356686</v>
@@ -32088,10 +32088,10 @@
     </row>
     <row r="106">
       <c r="A106" s="0" t="n">
-        <v>1088.49850521305</v>
+        <v>410.5615003133146</v>
       </c>
       <c r="B106" s="0" t="n">
-        <v>1229.586365848417</v>
+        <v>710.5074405856157</v>
       </c>
       <c r="C106" s="0" t="n">
         <v>302.7263446882706</v>
@@ -32390,10 +32390,10 @@
     </row>
     <row r="107">
       <c r="A107" s="0" t="n">
-        <v>1122.17512471307</v>
+        <v>398.2404970020496</v>
       </c>
       <c r="B107" s="0" t="n">
-        <v>1267.628046187689</v>
+        <v>732.4895458562627</v>
       </c>
       <c r="C107" s="0" t="n">
         <v>293.6414882356686</v>
@@ -32692,10 +32692,10 @@
     </row>
     <row r="108">
       <c r="A108" s="0" t="n">
-        <v>1088.49850521305</v>
+        <v>410.5615003133146</v>
       </c>
       <c r="B108" s="0" t="n">
-        <v>1306.846682845956</v>
+        <v>755.1517466819</v>
       </c>
       <c r="C108" s="0" t="n">
         <v>302.7263446882706</v>
@@ -32994,10 +32994,10 @@
     </row>
     <row r="109">
       <c r="A109" s="0" t="n">
-        <v>1122.17512471307</v>
+        <v>398.2404970020496</v>
       </c>
       <c r="B109" s="0" t="n">
-        <v>1267.628046187689</v>
+        <v>778.5150842666445</v>
       </c>
       <c r="C109" s="0" t="n">
         <v>293.6414882356687</v>
@@ -33296,10 +33296,10 @@
     </row>
     <row r="110">
       <c r="A110" s="0" t="n">
-        <v>1156.893651662222</v>
+        <v>386.2892485812951</v>
       </c>
       <c r="B110" s="0" t="n">
-        <v>1229.586365848417</v>
+        <v>802.6012508000039</v>
       </c>
       <c r="C110" s="0" t="n">
         <v>302.7263446882707</v>
@@ -33598,10 +33598,10 @@
     </row>
     <row r="111">
       <c r="A111" s="0" t="n">
-        <v>1122.175124713071</v>
+        <v>398.2404970020497</v>
       </c>
       <c r="B111" s="0" t="n">
-        <v>1192.68632121797</v>
+        <v>827.4326095974529</v>
       </c>
       <c r="C111" s="0" t="n">
         <v>312.0922738777679</v>
@@ -33900,10 +33900,10 @@
     </row>
     <row r="112">
       <c r="A112" s="0" t="n">
-        <v>1088.49850521305</v>
+        <v>386.2892485812952</v>
       </c>
       <c r="B112" s="0" t="n">
-        <v>1229.586365848417</v>
+        <v>853.0322158641317</v>
       </c>
       <c r="C112" s="0" t="n">
         <v>321.7479718010467</v>
@@ -34202,10 +34202,10 @@
     </row>
     <row r="113">
       <c r="A113" s="0" t="n">
-        <v>1122.175124713071</v>
+        <v>398.2404970020497</v>
       </c>
       <c r="B113" s="0" t="n">
-        <v>1267.628046187689</v>
+        <v>879.4238381009422</v>
       </c>
       <c r="C113" s="0" t="n">
         <v>312.0922738777679</v>
@@ -34504,10 +34504,10 @@
     </row>
     <row r="114">
       <c r="A114" s="0" t="n">
-        <v>1156.893651662222</v>
+        <v>410.5615003133148</v>
       </c>
       <c r="B114" s="0" t="n">
-        <v>1229.586365848417</v>
+        <v>906.631980172921</v>
       </c>
       <c r="C114" s="0" t="n">
         <v>321.7479718010468</v>
@@ -34806,10 +34806,10 @@
     </row>
     <row r="115">
       <c r="A115" s="0" t="n">
-        <v>1192.686321217971</v>
+        <v>423.263698213626</v>
       </c>
       <c r="B115" s="0" t="n">
-        <v>1267.628046187689</v>
+        <v>879.4238381009424</v>
       </c>
       <c r="C115" s="0" t="n">
         <v>331.7024034969602</v>
@@ -35108,10 +35108,10 @@
     </row>
     <row r="116">
       <c r="A116" s="0" t="n">
-        <v>1229.586365848419</v>
+        <v>436.3588843297722</v>
       </c>
       <c r="B116" s="0" t="n">
-        <v>1229.586365848417</v>
+        <v>906.6319801729211</v>
       </c>
       <c r="C116" s="0" t="n">
         <v>321.7479718010468</v>
@@ -35410,10 +35410,10 @@
     </row>
     <row r="117">
       <c r="A117" s="0" t="n">
-        <v>1192.686321217971</v>
+        <v>449.8592171668402</v>
       </c>
       <c r="B117" s="0" t="n">
-        <v>1192.68632121797</v>
+        <v>879.4238381009425</v>
       </c>
       <c r="C117" s="0" t="n">
         <v>331.7024034969603</v>
@@ -35712,10 +35712,10 @@
     </row>
     <row r="118">
       <c r="A118" s="0" t="n">
-        <v>1229.586365848419</v>
+        <v>436.3588843297722</v>
       </c>
       <c r="B118" s="0" t="n">
-        <v>1229.586365848417</v>
+        <v>906.6319801729212</v>
       </c>
       <c r="C118" s="0" t="n">
         <v>321.7479718010469</v>
@@ -36014,10 +36014,10 @@
     </row>
     <row r="119">
       <c r="A119" s="0" t="n">
-        <v>1192.686321217971</v>
+        <v>423.2636982136261</v>
       </c>
       <c r="B119" s="0" t="n">
-        <v>1192.68632121797</v>
+        <v>934.6819040603754</v>
       </c>
       <c r="C119" s="0" t="n">
         <v>331.7024034969604</v>
@@ -36316,10 +36316,10 @@
     </row>
     <row r="120">
       <c r="A120" s="0" t="n">
-        <v>1156.893651662222</v>
+        <v>436.3588843297723</v>
       </c>
       <c r="B120" s="0" t="n">
-        <v>1229.586365848417</v>
+        <v>963.5996533139079</v>
       </c>
       <c r="C120" s="0" t="n">
         <v>341.9648113701094</v>
@@ -36618,10 +36618,10 @@
     </row>
     <row r="121">
       <c r="A121" s="0" t="n">
-        <v>1192.686321217971</v>
+        <v>449.8592171668403</v>
       </c>
       <c r="B121" s="0" t="n">
-        <v>1192.68632121797</v>
+        <v>993.4120772351081</v>
       </c>
       <c r="C121" s="0" t="n">
         <v>352.5447237721512</v>
@@ -36920,10 +36920,10 @@
     </row>
     <row r="122">
       <c r="A122" s="0" t="n">
-        <v>1229.586365848419</v>
+        <v>436.3588843297723</v>
       </c>
       <c r="B122" s="0" t="n">
-        <v>1156.893651662221</v>
+        <v>1024.146855805359</v>
       </c>
       <c r="C122" s="0" t="n">
         <v>341.9648113701095</v>
@@ -37222,10 +37222,10 @@
     </row>
     <row r="123">
       <c r="A123" s="0" t="n">
-        <v>1267.628046187691</v>
+        <v>423.2636982136261</v>
       </c>
       <c r="B123" s="0" t="n">
-        <v>1192.68632121797</v>
+        <v>993.4120772351083</v>
       </c>
       <c r="C123" s="0" t="n">
         <v>352.5447237721513</v>
@@ -37524,10 +37524,10 @@
     </row>
     <row r="124">
       <c r="A124" s="0" t="n">
-        <v>1229.586365848419</v>
+        <v>410.561500313315</v>
       </c>
       <c r="B124" s="0" t="n">
-        <v>1229.586365848417</v>
+        <v>1024.146855805359</v>
       </c>
       <c r="C124" s="0" t="n">
         <v>341.9648113701095</v>
@@ -37826,10 +37826,10 @@
     </row>
     <row r="125">
       <c r="A125" s="0" t="n">
-        <v>1267.628046187691</v>
+        <v>398.2404970020499</v>
       </c>
       <c r="B125" s="0" t="n">
-        <v>1267.62804618769</v>
+        <v>993.4120772351084</v>
       </c>
       <c r="C125" s="0" t="n">
         <v>352.5447237721513</v>
@@ -38128,10 +38128,10 @@
     </row>
     <row r="126">
       <c r="A126" s="0" t="n">
-        <v>1306.846682845958</v>
+        <v>386.2892485812954</v>
       </c>
       <c r="B126" s="0" t="n">
-        <v>1306.846682845956</v>
+        <v>963.5996533139083</v>
       </c>
       <c r="C126" s="0" t="n">
         <v>363.4519638486003</v>
@@ -38430,10 +38430,10 @@
     </row>
     <row r="127">
       <c r="A127" s="0" t="n">
-        <v>1267.628046187691</v>
+        <v>398.2404970020499</v>
       </c>
       <c r="B127" s="0" t="n">
-        <v>1347.278689203607</v>
+        <v>993.4120772351085</v>
       </c>
       <c r="C127" s="0" t="n">
         <v>374.6966586593376</v>
@@ -38732,10 +38732,10 @@
     </row>
     <row r="128">
       <c r="A128" s="0" t="n">
-        <v>1229.586365848419</v>
+        <v>386.2892485812955</v>
       </c>
       <c r="B128" s="0" t="n">
-        <v>1306.846682845956</v>
+        <v>1024.146855805359</v>
       </c>
       <c r="C128" s="0" t="n">
         <v>386.289248581296</v>
@@ -39034,10 +39034,10 @@
     </row>
     <row r="129">
       <c r="A129" s="0" t="n">
-        <v>1192.686321217972</v>
+        <v>398.24049700205</v>
       </c>
       <c r="B129" s="0" t="n">
-        <v>1347.278689203607</v>
+        <v>993.4120772351087</v>
       </c>
       <c r="C129" s="0" t="n">
         <v>374.6966586593377</v>
@@ -39336,10 +39336,10 @@
     </row>
     <row r="130">
       <c r="A130" s="0" t="n">
-        <v>1156.893651662222</v>
+        <v>386.2892485812955</v>
       </c>
       <c r="B130" s="0" t="n">
-        <v>1306.846682845956</v>
+        <v>1024.146855805359</v>
       </c>
       <c r="C130" s="0" t="n">
         <v>363.4519638486004</v>
@@ -39638,10 +39638,10 @@
     </row>
     <row r="131">
       <c r="A131" s="0" t="n">
-        <v>1122.175124713071</v>
+        <v>374.6966586593372</v>
       </c>
       <c r="B131" s="0" t="n">
-        <v>1347.278689203607</v>
+        <v>993.4120772351087</v>
       </c>
       <c r="C131" s="0" t="n">
         <v>352.5447237721514</v>
@@ -39940,10 +39940,10 @@
     </row>
     <row r="132">
       <c r="A132" s="0" t="n">
-        <v>1156.893651662222</v>
+        <v>386.2892485812956</v>
       </c>
       <c r="B132" s="0" t="n">
-        <v>1388.961605220029</v>
+        <v>1024.146855805359</v>
       </c>
       <c r="C132" s="0" t="n">
         <v>363.4519638486004</v>
@@ -40242,10 +40242,10 @@
     </row>
     <row r="133">
       <c r="A133" s="0" t="n">
-        <v>1192.686321217972</v>
+        <v>374.6966586593372</v>
       </c>
       <c r="B133" s="0" t="n">
-        <v>1431.934132288385</v>
+        <v>993.4120772351087</v>
       </c>
       <c r="C133" s="0" t="n">
         <v>352.5447237721515</v>
@@ -40544,10 +40544,10 @@
     </row>
     <row r="134">
       <c r="A134" s="0" t="n">
-        <v>1156.893651662222</v>
+        <v>363.4519638485999</v>
       </c>
       <c r="B134" s="0" t="n">
-        <v>1388.961605220029</v>
+        <v>1024.146855805359</v>
       </c>
       <c r="C134" s="0" t="n">
         <v>363.4519638486005</v>
@@ -40846,10 +40846,10 @@
     </row>
     <row r="135">
       <c r="A135" s="0" t="n">
-        <v>1192.686321217972</v>
+        <v>352.544723772151</v>
       </c>
       <c r="B135" s="0" t="n">
-        <v>1431.934132288385</v>
+        <v>993.4120772351087</v>
       </c>
       <c r="C135" s="0" t="n">
         <v>374.6966586593379</v>
@@ -41148,10 +41148,10 @@
     </row>
     <row r="136">
       <c r="A136" s="0" t="n">
-        <v>1156.893651662222</v>
+        <v>341.9648113701093</v>
       </c>
       <c r="B136" s="0" t="n">
-        <v>1388.961605220029</v>
+        <v>1024.146855805359</v>
       </c>
       <c r="C136" s="0" t="n">
         <v>386.2892485812962</v>
@@ -41450,10 +41450,10 @@
     </row>
     <row r="137">
       <c r="A137" s="0" t="n">
-        <v>1192.686321217972</v>
+        <v>331.7024034969602</v>
       </c>
       <c r="B137" s="0" t="n">
-        <v>1347.278689203607</v>
+        <v>993.4120772351087</v>
       </c>
       <c r="C137" s="0" t="n">
         <v>374.6966586593379</v>
@@ -41752,10 +41752,10 @@
     </row>
     <row r="138">
       <c r="A138" s="0" t="n">
-        <v>1229.586365848419</v>
+        <v>341.9648113701093</v>
       </c>
       <c r="B138" s="0" t="n">
-        <v>1306.846682845957</v>
+        <v>963.5996533139086</v>
       </c>
       <c r="C138" s="0" t="n">
         <v>386.2892485812962</v>
@@ -42054,10 +42054,10 @@
     </row>
     <row r="139">
       <c r="A139" s="0" t="n">
-        <v>1267.628046187691</v>
+        <v>331.7024034969602</v>
       </c>
       <c r="B139" s="0" t="n">
-        <v>1267.62804618769</v>
+        <v>934.6819040603762</v>
       </c>
       <c r="C139" s="0" t="n">
         <v>398.2404970020508</v>
@@ -42356,10 +42356,10 @@
     </row>
     <row r="140">
       <c r="A140" s="0" t="n">
-        <v>1306.846682845958</v>
+        <v>341.9648113701093</v>
       </c>
       <c r="B140" s="0" t="n">
-        <v>1306.846682845957</v>
+        <v>963.5996533139087</v>
       </c>
       <c r="C140" s="0" t="n">
         <v>386.2892485812963</v>
@@ -42658,10 +42658,10 @@
     </row>
     <row r="141">
       <c r="A141" s="0" t="n">
-        <v>1347.278689203609</v>
+        <v>331.7024034969602</v>
       </c>
       <c r="B141" s="0" t="n">
-        <v>1347.278689203607</v>
+        <v>993.4120772351089</v>
       </c>
       <c r="C141" s="0" t="n">
         <v>398.2404970020509</v>
@@ -42960,10 +42960,10 @@
     </row>
     <row r="142">
       <c r="A142" s="0" t="n">
-        <v>1388.961605220031</v>
+        <v>321.7479718010468</v>
       </c>
       <c r="B142" s="0" t="n">
-        <v>1306.846682845957</v>
+        <v>1024.146855805359</v>
       </c>
       <c r="C142" s="0" t="n">
         <v>386.2892485812964</v>
@@ -43262,10 +43262,10 @@
     </row>
     <row r="143">
       <c r="A143" s="0" t="n">
-        <v>1431.934132288387</v>
+        <v>331.7024034969602</v>
       </c>
       <c r="B143" s="0" t="n">
-        <v>1347.278689203607</v>
+        <v>993.4120772351089</v>
       </c>
       <c r="C143" s="0" t="n">
         <v>374.696658659338</v>
@@ -43564,10 +43564,10 @@
     </row>
     <row r="144">
       <c r="A144" s="0" t="n">
-        <v>1476.236169168749</v>
+        <v>341.9648113701093</v>
       </c>
       <c r="B144" s="0" t="n">
-        <v>1306.846682845957</v>
+        <v>1024.146855805359</v>
       </c>
       <c r="C144" s="0" t="n">
         <v>386.2892485812964</v>
@@ -43866,10 +43866,10 @@
     </row>
     <row r="145">
       <c r="A145" s="0" t="n">
-        <v>1521.908849032957</v>
+        <v>331.7024034969602</v>
       </c>
       <c r="B145" s="0" t="n">
-        <v>1267.62804618769</v>
+        <v>993.4120772351089</v>
       </c>
       <c r="C145" s="0" t="n">
         <v>398.2404970020509</v>
@@ -44168,10 +44168,10 @@
     </row>
     <row r="146">
       <c r="A146" s="0" t="n">
-        <v>1476.236169168749</v>
+        <v>341.9648113701093</v>
       </c>
       <c r="B146" s="0" t="n">
-        <v>1306.846682845957</v>
+        <v>1024.146855805359</v>
       </c>
       <c r="C146" s="0" t="n">
         <v>386.2892485812964</v>
@@ -44470,10 +44470,10 @@
     </row>
     <row r="147">
       <c r="A147" s="0" t="n">
-        <v>1521.908849032957</v>
+        <v>331.7024034969602</v>
       </c>
       <c r="B147" s="0" t="n">
-        <v>1267.62804618769</v>
+        <v>1055.832525385906</v>
       </c>
       <c r="C147" s="0" t="n">
         <v>374.696658659338</v>
@@ -44772,10 +44772,10 @@
     </row>
     <row r="148">
       <c r="A148" s="0" t="n">
-        <v>1476.236169168749</v>
+        <v>321.7479718010468</v>
       </c>
       <c r="B148" s="0" t="n">
-        <v>1306.846682845957</v>
+        <v>1024.14685580536</v>
       </c>
       <c r="C148" s="0" t="n">
         <v>386.2892485812964</v>
@@ -45074,10 +45074,10 @@
     </row>
     <row r="149">
       <c r="A149" s="0" t="n">
-        <v>1431.934132288387</v>
+        <v>331.7024034969603</v>
       </c>
       <c r="B149" s="0" t="n">
-        <v>1267.62804618769</v>
+        <v>993.4120772351091</v>
       </c>
       <c r="C149" s="0" t="n">
         <v>374.696658659338</v>
@@ -45376,10 +45376,10 @@
     </row>
     <row r="150">
       <c r="A150" s="0" t="n">
-        <v>1388.961605220031</v>
+        <v>321.7479718010469</v>
       </c>
       <c r="B150" s="0" t="n">
-        <v>1306.846682845957</v>
+        <v>1024.14685580536</v>
       </c>
       <c r="C150" s="0" t="n">
         <v>386.2892485812964</v>
@@ -45678,10 +45678,10 @@
     </row>
     <row r="151">
       <c r="A151" s="0" t="n">
-        <v>1431.934132288387</v>
+        <v>331.7024034969604</v>
       </c>
       <c r="B151" s="0" t="n">
-        <v>1347.278689203607</v>
+        <v>993.4120772351091</v>
       </c>
       <c r="C151" s="0" t="n">
         <v>398.240497002051</v>
@@ -45980,10 +45980,10 @@
     </row>
     <row r="152">
       <c r="A152" s="0" t="n">
-        <v>1476.23616916875</v>
+        <v>321.747971801047</v>
       </c>
       <c r="B152" s="0" t="n">
-        <v>1306.846682845957</v>
+        <v>1024.14685580536</v>
       </c>
       <c r="C152" s="0" t="n">
         <v>410.5615003133161</v>
@@ -46282,10 +46282,10 @@
     </row>
     <row r="153">
       <c r="A153" s="0" t="n">
-        <v>1431.934132288387</v>
+        <v>331.7024034969604</v>
       </c>
       <c r="B153" s="0" t="n">
-        <v>1267.62804618769</v>
+        <v>993.4120772351091</v>
       </c>
       <c r="C153" s="0" t="n">
         <v>423.2636982136273</v>
@@ -46584,10 +46584,10 @@
     </row>
     <row r="154">
       <c r="A154" s="0" t="n">
-        <v>1388.961605220032</v>
+        <v>321.747971801047</v>
       </c>
       <c r="B154" s="0" t="n">
-        <v>1306.846682845957</v>
+        <v>963.599653313909</v>
       </c>
       <c r="C154" s="0" t="n">
         <v>410.5615003133161</v>
@@ -46886,10 +46886,10 @@
     </row>
     <row r="155">
       <c r="A155" s="0" t="n">
-        <v>1431.934132288387</v>
+        <v>312.0922738777682</v>
       </c>
       <c r="B155" s="0" t="n">
-        <v>1347.278689203607</v>
+        <v>993.4120772351092</v>
       </c>
       <c r="C155" s="0" t="n">
         <v>423.2636982136273</v>
@@ -47188,10 +47188,10 @@
     </row>
     <row r="156">
       <c r="A156" s="0" t="n">
-        <v>1476.23616916875</v>
+        <v>302.7263446882711</v>
       </c>
       <c r="B156" s="0" t="n">
-        <v>1388.961605220029</v>
+        <v>1024.14685580536</v>
       </c>
       <c r="C156" s="0" t="n">
         <v>410.5615003133161</v>
@@ -47490,10 +47490,10 @@
     </row>
     <row r="157">
       <c r="A157" s="0" t="n">
-        <v>1431.934132288387</v>
+        <v>293.6414882356691</v>
       </c>
       <c r="B157" s="0" t="n">
-        <v>1431.934132288385</v>
+        <v>1055.832525385906</v>
       </c>
       <c r="C157" s="0" t="n">
         <v>423.2636982136273</v>
@@ -47792,10 +47792,10 @@
     </row>
     <row r="158">
       <c r="A158" s="0" t="n">
-        <v>1388.961605220032</v>
+        <v>284.8292694910584</v>
       </c>
       <c r="B158" s="0" t="n">
-        <v>1388.961605220029</v>
+        <v>1088.498505213051</v>
       </c>
       <c r="C158" s="0" t="n">
         <v>410.5615003133161</v>
@@ -48094,10 +48094,10 @@
     </row>
     <row r="159">
       <c r="A159" s="0" t="n">
-        <v>1347.27868920361</v>
+        <v>276.2815065618349</v>
       </c>
       <c r="B159" s="0" t="n">
-        <v>1347.278689203608</v>
+        <v>1055.832525385907</v>
       </c>
       <c r="C159" s="0" t="n">
         <v>398.240497002051</v>
@@ -48396,10 +48396,10 @@
     </row>
     <row r="160">
       <c r="A160" s="0" t="n">
-        <v>1388.961605220032</v>
+        <v>284.8292694910585</v>
       </c>
       <c r="B160" s="0" t="n">
-        <v>1306.846682845957</v>
+        <v>1088.498505213052</v>
       </c>
       <c r="C160" s="0" t="n">
         <v>386.2892485812965</v>
@@ -48698,10 +48698,10 @@
     </row>
     <row r="161">
       <c r="A161" s="0" t="n">
-        <v>1347.27868920361</v>
+        <v>276.281506561835</v>
       </c>
       <c r="B161" s="0" t="n">
-        <v>1267.62804618769</v>
+        <v>1122.175124713072</v>
       </c>
       <c r="C161" s="0" t="n">
         <v>398.240497002051</v>
@@ -49000,10 +49000,10 @@
     </row>
     <row r="162">
       <c r="A162" s="0" t="n">
-        <v>1306.84668284596</v>
+        <v>267.9902630950416</v>
       </c>
       <c r="B162" s="0" t="n">
-        <v>1229.586365848418</v>
+        <v>1088.498505213052</v>
       </c>
       <c r="C162" s="0" t="n">
         <v>410.5615003133162</v>
@@ -49302,10 +49302,10 @@
     </row>
     <row r="163">
       <c r="A163" s="0" t="n">
-        <v>1267.628046187693</v>
+        <v>259.9478409086919</v>
       </c>
       <c r="B163" s="0" t="n">
-        <v>1192.686321217971</v>
+        <v>1055.832525385907</v>
       </c>
       <c r="C163" s="0" t="n">
         <v>423.2636982136274</v>
@@ -49604,10 +49604,10 @@
     </row>
     <row r="164">
       <c r="A164" s="0" t="n">
-        <v>1229.586365848421</v>
+        <v>267.9902630950416</v>
       </c>
       <c r="B164" s="0" t="n">
-        <v>1229.586365848418</v>
+        <v>1024.14685580536</v>
       </c>
       <c r="C164" s="0" t="n">
         <v>436.3588843297736</v>
@@ -49906,10 +49906,10 @@
     </row>
     <row r="165">
       <c r="A165" s="0" t="n">
-        <v>1192.686321217973</v>
+        <v>276.281506561835</v>
       </c>
       <c r="B165" s="0" t="n">
-        <v>1192.686321217971</v>
+        <v>993.41207723511</v>
       </c>
       <c r="C165" s="0" t="n">
         <v>423.2636982136274</v>
@@ -50208,10 +50208,10 @@
     </row>
     <row r="166">
       <c r="A166" s="0" t="n">
-        <v>1156.893651662224</v>
+        <v>284.8292694910586</v>
       </c>
       <c r="B166" s="0" t="n">
-        <v>1156.893651662222</v>
+        <v>963.5996533139099</v>
       </c>
       <c r="C166" s="0" t="n">
         <v>436.3588843297737</v>
@@ -50510,10 +50510,10 @@
     </row>
     <row r="167">
       <c r="A167" s="0" t="n">
-        <v>1122.175124713073</v>
+        <v>293.6414882356693</v>
       </c>
       <c r="B167" s="0" t="n">
-        <v>1122.175124713071</v>
+        <v>993.4120772351101</v>
       </c>
       <c r="C167" s="0" t="n">
         <v>449.8592171668417</v>
@@ -50812,10 +50812,10 @@
     </row>
     <row r="168">
       <c r="A168" s="0" t="n">
-        <v>1156.893651662224</v>
+        <v>302.7263446882713</v>
       </c>
       <c r="B168" s="0" t="n">
-        <v>1156.893651662222</v>
+        <v>1024.146855805361</v>
       </c>
       <c r="C168" s="0" t="n">
         <v>436.3588843297737</v>
@@ -51114,10 +51114,10 @@
     </row>
     <row r="169">
       <c r="A169" s="0" t="n">
-        <v>1192.686321217974</v>
+        <v>312.0922738777685</v>
       </c>
       <c r="B169" s="0" t="n">
-        <v>1122.175124713071</v>
+        <v>993.4120772351102</v>
       </c>
       <c r="C169" s="0" t="n">
         <v>423.2636982136275</v>
@@ -51416,10 +51416,10 @@
     </row>
     <row r="170">
       <c r="A170" s="0" t="n">
-        <v>1229.586365848421</v>
+        <v>302.7263446882713</v>
       </c>
       <c r="B170" s="0" t="n">
-        <v>1156.893651662222</v>
+        <v>963.59965331391</v>
       </c>
       <c r="C170" s="0" t="n">
         <v>436.3588843297738</v>
@@ -51718,10 +51718,10 @@
     </row>
     <row r="171">
       <c r="A171" s="0" t="n">
-        <v>1267.628046187693</v>
+        <v>293.6414882356693</v>
       </c>
       <c r="B171" s="0" t="n">
-        <v>1122.175124713071</v>
+        <v>934.6819040603775</v>
       </c>
       <c r="C171" s="0" t="n">
         <v>423.2636982136276</v>
@@ -52020,10 +52020,10 @@
     </row>
     <row r="172">
       <c r="A172" s="0" t="n">
-        <v>1306.84668284596</v>
+        <v>284.8292694910587</v>
       </c>
       <c r="B172" s="0" t="n">
-        <v>1088.49850521305</v>
+        <v>963.5996533139102</v>
       </c>
       <c r="C172" s="0" t="n">
         <v>410.5615003133164</v>
@@ -52322,10 +52322,10 @@
     </row>
     <row r="173">
       <c r="A173" s="0" t="n">
-        <v>1267.628046187693</v>
+        <v>293.6414882356694</v>
       </c>
       <c r="B173" s="0" t="n">
-        <v>1055.832525385905</v>
+        <v>993.4120772351104</v>
       </c>
       <c r="C173" s="0" t="n">
         <v>423.2636982136276</v>
@@ -52624,10 +52624,10 @@
     </row>
     <row r="174">
       <c r="A174" s="0" t="n">
-        <v>1306.84668284596</v>
+        <v>302.7263446882714</v>
       </c>
       <c r="B174" s="0" t="n">
-        <v>1024.146855805359</v>
+        <v>1024.146855805361</v>
       </c>
       <c r="C174" s="0" t="n">
         <v>436.3588843297738</v>
@@ -52926,10 +52926,10 @@
     </row>
     <row r="175">
       <c r="A175" s="0" t="n">
-        <v>1267.628046187694</v>
+        <v>312.0922738777685</v>
       </c>
       <c r="B175" s="0" t="n">
-        <v>993.4120772351084</v>
+        <v>993.4120772351105</v>
       </c>
       <c r="C175" s="0" t="n">
         <v>423.2636982136277</v>
@@ -53228,10 +53228,10 @@
     </row>
     <row r="176">
       <c r="A176" s="0" t="n">
-        <v>1229.586365848422</v>
+        <v>302.7263446882714</v>
       </c>
       <c r="B176" s="0" t="n">
-        <v>1024.146855805359</v>
+        <v>1024.146855805361</v>
       </c>
       <c r="C176" s="0" t="n">
         <v>436.3588843297739</v>
@@ -53530,10 +53530,10 @@
     </row>
     <row r="177">
       <c r="A177" s="0" t="n">
-        <v>1267.628046187694</v>
+        <v>312.0922738777685</v>
       </c>
       <c r="B177" s="0" t="n">
-        <v>993.4120772351084</v>
+        <v>993.4120772351107</v>
       </c>
       <c r="C177" s="0" t="n">
         <v>449.859217166842</v>
@@ -53832,10 +53832,10 @@
     </row>
     <row r="178">
       <c r="A178" s="0" t="n">
-        <v>1306.846682845961</v>
+        <v>302.7263446882714</v>
       </c>
       <c r="B178" s="0" t="n">
-        <v>1024.146855805359</v>
+        <v>1024.146855805361</v>
       </c>
       <c r="C178" s="0" t="n">
         <v>463.7772313970403</v>
@@ -54134,10 +54134,10 @@
     </row>
     <row r="179">
       <c r="A179" s="0" t="n">
-        <v>1347.278689203612</v>
+        <v>312.0922738777685</v>
       </c>
       <c r="B179" s="0" t="n">
-        <v>1055.832525385905</v>
+        <v>993.4120772351109</v>
       </c>
       <c r="C179" s="0" t="n">
         <v>449.859217166842</v>
@@ -54436,10 +54436,10 @@
     </row>
     <row r="180">
       <c r="A180" s="0" t="n">
-        <v>1306.846682845961</v>
+        <v>302.7263446882714</v>
       </c>
       <c r="B180" s="0" t="n">
-        <v>1024.146855805359</v>
+        <v>1024.146855805362</v>
       </c>
       <c r="C180" s="0" t="n">
         <v>463.7772313970403</v>

</xml_diff>